<commit_message>
minor improvements & more results
</commit_message>
<xml_diff>
--- a/Saved Times.xlsx
+++ b/Saved Times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.comerford\source\repos\Threading_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B7EA54-B59E-4033-97EC-EF95021F7FD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE2909E-FADF-4D02-BB80-E5465B3BD3FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Matrix Size</t>
   </si>
@@ -51,25 +51,22 @@
     <t>Non threaded</t>
   </si>
   <si>
-    <t>2x2: 0.022118</t>
-  </si>
-  <si>
-    <t>4x4: 0.249332</t>
-  </si>
-  <si>
-    <t>8x8: 1.40316</t>
-  </si>
-  <si>
-    <t>16x16: 9.57151</t>
-  </si>
-  <si>
-    <t>32x32: 57.5556</t>
-  </si>
-  <si>
-    <t>64x64: 368.309</t>
-  </si>
-  <si>
-    <t>128x128: 3045.05</t>
+    <t>2x2</t>
+  </si>
+  <si>
+    <t>Threaded (v1)</t>
+  </si>
+  <si>
+    <t>Threaded(v1 unrolled)</t>
+  </si>
+  <si>
+    <t>512x512</t>
+  </si>
+  <si>
+    <t>Single Run</t>
+  </si>
+  <si>
+    <t>avg(50 runs)</t>
   </si>
 </sst>
 </file>
@@ -85,12 +82,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,8 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,110 +412,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A15"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1.4426E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>10.369400000000001</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3.0756700000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>8.1960000000000005E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="4">
+        <v>0.15612799999999999</v>
+      </c>
+      <c r="C3" s="4">
+        <v>7.4954999999999998</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5.0055500000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0.75488</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="4">
+        <v>1.1719999999999999</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5.6557399999999998</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5.7905100000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>5.8070300000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="4">
+        <v>9.3859100000000009</v>
+      </c>
+      <c r="C5" s="4">
+        <v>12.015499999999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>15.3978</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>53.2605</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="4">
+        <v>44.476100000000002</v>
+      </c>
+      <c r="C6" s="4">
+        <v>34.9758</v>
+      </c>
+      <c r="D6" s="4">
+        <v>29.6067</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>363.71199999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="4">
+        <v>367.73700000000002</v>
+      </c>
+      <c r="C7" s="4">
+        <v>173.006</v>
+      </c>
+      <c r="D7" s="4">
+        <v>172.87700000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>3088.92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B8" s="4">
+        <v>2824.61</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1407.51</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1334.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B10" s="1">
+        <v>189640</v>
+      </c>
+      <c r="C10" s="1">
+        <v>96969.600000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>